<commit_message>
practice: Solve Leetcode Problem#415 Add Strings
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1D55FE-D6BF-A84A-BE2F-610D3334795B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21280" windowHeight="16360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,157 +25,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="42">
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
   <si>
     <t xml:space="preserve"> Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeetCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Two Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephan</t>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>1. Two Sum</t>
+  </si>
+  <si>
+    <t>2020/11/17</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Stephan</t>
   </si>
   <si>
     <t xml:space="preserve">206. Reverse Linked List </t>
   </si>
   <si>
-    <t xml:space="preserve">2020/11/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linked List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To attempt recursive method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">937. Reorder Data in Log Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incomplete</t>
+    <t>2020/11/18</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>To attempt recursive method</t>
+  </si>
+  <si>
+    <t>937. Reorder Data in Log Files</t>
+  </si>
+  <si>
+    <t>2020/11/20</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
   <si>
     <t xml:space="preserve">Completed.  Good reference: [Sort an Array of objects](https://www.sitepoint.com/sort-an-array-of-objects-in-javascript/) </t>
   </si>
   <si>
-    <t xml:space="preserve">53. Maximum Subarray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21. Merge Two Sorted Lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array, DP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stocl</t>
+    <t>53. Maximum Subarray</t>
+  </si>
+  <si>
+    <t>2020/11/23</t>
+  </si>
+  <si>
+    <t>21. Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>2020/11/24</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>2020/12/01</t>
+  </si>
+  <si>
+    <t>Array, DP</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stocl</t>
   </si>
   <si>
     <t xml:space="preserve">199/200 Test Cases </t>
   </si>
   <si>
-    <t xml:space="preserve">953. Verifying an Alien Dictionary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hash Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. Generate Parentheses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String, Stack</t>
+    <t>953. Verifying an Alien Dictionary</t>
+  </si>
+  <si>
+    <t>2020/12/02</t>
+  </si>
+  <si>
+    <t>Hash Table</t>
+  </si>
+  <si>
+    <t>2020/12/04</t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses</t>
+  </si>
+  <si>
+    <t>2020/12/07</t>
+  </si>
+  <si>
+    <t>String, Stack</t>
+  </si>
+  <si>
+    <t>415. Add Strings</t>
+  </si>
+  <si>
+    <t>2020/12/08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,7 +174,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -190,87 +182,350 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.01"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -293,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -316,7 +571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -339,7 +594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -362,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -385,7 +640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -408,7 +663,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -431,7 +686,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -454,7 +709,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -477,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -486,7 +741,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -509,7 +764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -532,14 +787,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -548,21 +803,21 @@
       <c r="E13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -578,14 +833,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -594,21 +849,21 @@
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -624,33 +879,56 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>9</v>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#7 Reverse Integer
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C5307B-7163-DC43-B860-8EA8282E1D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,172 +25,153 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="45">
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
   <si>
     <t xml:space="preserve"> Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeetCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Two Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephan</t>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>1. Two Sum</t>
+  </si>
+  <si>
+    <t>2020/11/17</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Stephan</t>
   </si>
   <si>
     <t xml:space="preserve">206. Reverse Linked List </t>
   </si>
   <si>
-    <t xml:space="preserve">2020/11/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linked List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To attempt recursive method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">937. Reorder Data in Log Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incomplete</t>
+    <t>2020/11/18</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>To attempt recursive method</t>
+  </si>
+  <si>
+    <t>937. Reorder Data in Log Files</t>
+  </si>
+  <si>
+    <t>2020/11/20</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
   <si>
     <t xml:space="preserve">Completed.  Good reference: [Sort an Array of objects](https://www.sitepoint.com/sort-an-array-of-objects-in-javascript/) </t>
   </si>
   <si>
-    <t xml:space="preserve">53. Maximum Subarray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21. Merge Two Sorted Lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array, DP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stocl</t>
+    <t>53. Maximum Subarray</t>
+  </si>
+  <si>
+    <t>2020/11/23</t>
+  </si>
+  <si>
+    <t>21. Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>2020/11/24</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>2020/12/01</t>
+  </si>
+  <si>
+    <t>Array, DP</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stocl</t>
   </si>
   <si>
     <t xml:space="preserve">199/200 Test Cases </t>
   </si>
   <si>
-    <t xml:space="preserve">953. Verifying an Alien Dictionary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hash Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. Generate Parentheses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String, Stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">415. Add Strings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/08</t>
+    <t>953. Verifying an Alien Dictionary</t>
+  </si>
+  <si>
+    <t>2020/12/02</t>
+  </si>
+  <si>
+    <t>Hash Table</t>
+  </si>
+  <si>
+    <t>2020/12/04</t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses</t>
+  </si>
+  <si>
+    <t>2020/12/07</t>
+  </si>
+  <si>
+    <t>String, Stack</t>
+  </si>
+  <si>
+    <t>415. Add Strings</t>
+  </si>
+  <si>
+    <t>2020/12/08</t>
   </si>
   <si>
     <t xml:space="preserve">7. Reverse Integer </t>
   </si>
   <si>
-    <t xml:space="preserve">2020/12/09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math</t>
+    <t>2020/12/09</t>
+  </si>
+  <si>
+    <t>Math</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -202,7 +188,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -210,91 +196,351 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21:C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.01"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -317,7 +563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -340,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -363,7 +609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -386,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -409,7 +655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -432,7 +678,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -455,7 +701,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -478,7 +724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -501,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -510,7 +756,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -533,7 +779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -556,14 +802,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -572,21 +818,21 @@
       <c r="E13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -602,14 +848,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -618,21 +864,21 @@
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -648,14 +894,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -671,14 +917,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -694,14 +940,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -710,21 +956,21 @@
       <c r="E19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="6" t="s">
@@ -736,34 +982,36 @@
       <c r="F20" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Practice: Solve Leetcode Problem#88: Merge Sorted Array
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C5307B-7163-DC43-B860-8EA8282E1D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8681FD47-13DA-624F-B3EE-C7A93B522406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
   <si>
     <t>Site</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Math</t>
+  </si>
+  <si>
+    <t>88. Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>2020/12/14</t>
+  </si>
+  <si>
+    <t>Array, Merge</t>
+  </si>
+  <si>
+    <t>176. Second Highest Salary</t>
+  </si>
+  <si>
+    <t>2020/12/</t>
   </si>
 </sst>
 </file>
@@ -527,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -986,7 +1001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -996,8 +1011,14 @@
       <c r="C21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -1007,6 +1028,52 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem# 176 Second Highest Salary
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8681FD47-13DA-624F-B3EE-C7A93B522406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E050E-CF4F-9C4E-99F4-649DE5508A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
   <si>
     <t>Site</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>2020/12/</t>
+  </si>
+  <si>
+    <t>SQL</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1054,6 +1057,9 @@
       <c r="D23" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
@@ -1069,11 +1075,37 @@
         <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
       <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Practice: Solve Leetcode Problem#234 Palindrome Linked List
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E050E-CF4F-9C4E-99F4-649DE5508A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA3C66B-9064-D04C-AC40-ED8E8C513C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
   <si>
     <t>Site</t>
   </si>
@@ -174,10 +174,16 @@
     <t>176. Second Highest Salary</t>
   </si>
   <si>
-    <t>2020/12/</t>
-  </si>
-  <si>
     <t>SQL</t>
+  </si>
+  <si>
+    <t>234. Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>2020/12/15</t>
+  </si>
+  <si>
+    <t>Lindked List</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1017,9 +1023,6 @@
       <c r="D21" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
@@ -1057,9 +1060,6 @@
       <c r="D23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
@@ -1078,25 +1078,27 @@
         <v>46</v>
       </c>
       <c r="F24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1105,6 +1107,18 @@
       </c>
       <c r="C26" t="s">
         <v>9</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Practice: Solve Leetcode Problem#155 Min Stack
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA3C66B-9064-D04C-AC40-ED8E8C513C6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7102313-E3E5-8641-843D-25B5129E426F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="56">
   <si>
     <t>Site</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>Lindked List</t>
+  </si>
+  <si>
+    <t>155. Min Stack</t>
+  </si>
+  <si>
+    <t>2020/12/16</t>
+  </si>
+  <si>
+    <t>Stack</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1121,6 +1130,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Practice: Leetcode Problem#14 Longest Common Prefix
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7102313-E3E5-8641-843D-25B5129E426F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3729EF51-7D7A-1643-8B43-3FBD378F392C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24440" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="59">
   <si>
     <t>Site</t>
   </si>
@@ -193,6 +193,15 @@
   </si>
   <si>
     <t>Stack</t>
+  </si>
+  <si>
+    <t>14. Longest Common Prefix</t>
+  </si>
+  <si>
+    <t>2020/12/17</t>
+  </si>
+  <si>
+    <t>Sring</t>
   </si>
 </sst>
 </file>
@@ -560,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1151,6 +1160,9 @@
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
       <c r="D28" s="4" t="s">
         <v>53</v>
       </c>
@@ -1161,6 +1173,29 @@
         <v>55</v>
       </c>
       <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#283 Move Zeroes
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0B1D95-C418-F84A-B846-B2384B820DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,220 +25,207 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="61">
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="63">
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
   <si>
     <t xml:space="preserve"> Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LeetCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Two Sum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephan</t>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>LeetCode</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>1. Two Sum</t>
+  </si>
+  <si>
+    <t>2020/11/17</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Stephan</t>
   </si>
   <si>
     <t xml:space="preserve">206. Reverse Linked List </t>
   </si>
   <si>
-    <t xml:space="preserve">2020/11/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linked List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To attempt recursive method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">937. Reorder Data in Log Files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incomplete</t>
+    <t>2020/11/18</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>To attempt recursive method</t>
+  </si>
+  <si>
+    <t>937. Reorder Data in Log Files</t>
+  </si>
+  <si>
+    <t>2020/11/20</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
   <si>
     <t xml:space="preserve">Completed.  Good reference: [Sort an Array of objects](https://www.sitepoint.com/sort-an-array-of-objects-in-javascript/) </t>
   </si>
   <si>
-    <t xml:space="preserve">53. Maximum Subarray</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21. Merge Two Sorted Lists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/11/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array, DP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">121. Best Time to Buy and Sell Stocl</t>
+    <t>53. Maximum Subarray</t>
+  </si>
+  <si>
+    <t>2020/11/23</t>
+  </si>
+  <si>
+    <t>21. Merge Two Sorted Lists</t>
+  </si>
+  <si>
+    <t>2020/11/24</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stock</t>
+  </si>
+  <si>
+    <t>2020/12/01</t>
+  </si>
+  <si>
+    <t>Array, DP</t>
+  </si>
+  <si>
+    <t>121. Best Time to Buy and Sell Stocl</t>
   </si>
   <si>
     <t xml:space="preserve">199/200 Test Cases </t>
   </si>
   <si>
-    <t xml:space="preserve">953. Verifying an Alien Dictionary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hash Table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. Generate Parentheses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String, Stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">415. Add Strings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/08</t>
+    <t>953. Verifying an Alien Dictionary</t>
+  </si>
+  <si>
+    <t>2020/12/02</t>
+  </si>
+  <si>
+    <t>Hash Table</t>
+  </si>
+  <si>
+    <t>2020/12/04</t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses</t>
+  </si>
+  <si>
+    <t>2020/12/07</t>
+  </si>
+  <si>
+    <t>String, Stack</t>
+  </si>
+  <si>
+    <t>415. Add Strings</t>
+  </si>
+  <si>
+    <t>2020/12/08</t>
   </si>
   <si>
     <t xml:space="preserve">7. Reverse Integer </t>
   </si>
   <si>
-    <t xml:space="preserve">2020/12/09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88. Merge Sorted Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array, Merge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">176. Second Highest Salary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">234. Palindrome Linked List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lindked List</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">155. Min Stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14. Longest Common Prefix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020/12/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sring</t>
+    <t>2020/12/09</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>88. Merge Sorted Array</t>
+  </si>
+  <si>
+    <t>2020/12/18</t>
+  </si>
+  <si>
+    <t>Array, Merge</t>
+  </si>
+  <si>
+    <t>2020/12/14</t>
+  </si>
+  <si>
+    <t>176. Second Highest Salary</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>234. Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>Lindked List</t>
+  </si>
+  <si>
+    <t>2020/12/15</t>
+  </si>
+  <si>
+    <t>155. Min Stack</t>
+  </si>
+  <si>
+    <t>2020/12/16</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>14. Longest Common Prefix</t>
+  </si>
+  <si>
+    <t>2020/12/17</t>
+  </si>
+  <si>
+    <t>Sring</t>
   </si>
   <si>
     <t xml:space="preserve">283. Move Zeroes </t>
+  </si>
+  <si>
+    <t>2020/12/21</t>
+  </si>
+  <si>
+    <t>1480. Running Sum of  1d Array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,7 +237,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -253,87 +245,350 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.01"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -356,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -379,7 +634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -402,7 +657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -425,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -448,7 +703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -471,7 +726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -494,7 +749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -517,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -540,7 +795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -549,7 +804,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -572,7 +827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -595,14 +850,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -611,21 +866,21 @@
       <c r="E13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -641,14 +896,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -657,21 +912,21 @@
       <c r="E15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -687,14 +942,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -710,14 +965,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -733,14 +988,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -749,21 +1004,21 @@
       <c r="E19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -775,18 +1030,18 @@
       <c r="F20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -798,18 +1053,18 @@
       <c r="F21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -821,18 +1076,18 @@
       <c r="F22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -841,21 +1096,21 @@
       <c r="E23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -864,21 +1119,21 @@
       <c r="E24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="F24" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -887,21 +1142,21 @@
       <c r="E25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="F25" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -910,35 +1165,35 @@
       <c r="E26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="0" t="s">
+      <c r="F26" t="s">
         <v>52</v>
       </c>
-      <c r="G26" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -947,36 +1202,36 @@
       <c r="E28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="0" t="s">
+      <c r="F28" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -985,90 +1240,101 @@
       <c r="E30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="0" t="s">
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="G30" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#1480 Running Sum of 1d array
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0B1D95-C418-F84A-B846-B2384B820DCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FFFB73-3D1D-594D-8B48-E3EE8478DA2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="63">
   <si>
     <t>Site</t>
   </si>
@@ -578,7 +578,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:G34"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1281,7 +1281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -1308,8 +1308,14 @@
       <c r="D34" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1320,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Practice: Solve Leetcode Problem#706 Design HashMap
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FFFB73-3D1D-594D-8B48-E3EE8478DA2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1878B35C-AE0B-AD4E-A6E1-CC00FCD676CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="65">
   <si>
     <t>Site</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>1480. Running Sum of  1d Array</t>
+  </si>
+  <si>
+    <t>706. Design HashMap</t>
+  </si>
+  <si>
+    <t>2020/12/23</t>
   </si>
 </sst>
 </file>
@@ -575,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1315,7 +1321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1325,8 +1331,11 @@
       <c r="C35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D35" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -1334,6 +1343,37 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#13 Roman To Integer
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1878B35C-AE0B-AD4E-A6E1-CC00FCD676CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC089F6-3BCC-3A4E-82A7-C8AD575B703F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="67">
   <si>
     <t>Site</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>2020/12/23</t>
+  </si>
+  <si>
+    <t>13. Roman To Integer</t>
+  </si>
+  <si>
+    <t>2020/12/28</t>
   </si>
 </sst>
 </file>
@@ -581,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1355,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>7</v>
       </c>
@@ -1365,8 +1371,11 @@
       <c r="C37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="D37" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>7</v>
       </c>
@@ -1374,6 +1383,60 @@
         <v>14</v>
       </c>
       <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
range(1, len(nums)) in Python
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="72">
   <si>
     <t xml:space="preserve">Site</t>
   </si>
@@ -208,9 +208,15 @@
     <t xml:space="preserve">2020/12/21</t>
   </si>
   <si>
+    <t xml:space="preserve">Array, Two Pointers</t>
+  </si>
+  <si>
     <t xml:space="preserve">1480. Running Sum of  1d Array</t>
   </si>
   <si>
+    <t xml:space="preserve">2020/12/30</t>
+  </si>
+  <si>
     <t xml:space="preserve">706. Design HashMap</t>
   </si>
   <si>
@@ -221,6 +227,15 @@
   </si>
   <si>
     <t xml:space="preserve">2020/12/28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67. Add Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">680. Valid Palindrome II </t>
+  </si>
+  <si>
+    <t xml:space="preserve">453. Minimum Moves to Equal Array Elements</t>
   </si>
 </sst>
 </file>
@@ -338,17 +353,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -994,6 +1009,15 @@
       <c r="D29" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -1011,12 +1035,14 @@
       <c r="E30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="G30" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1030,7 +1056,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
@@ -1046,11 +1072,14 @@
       <c r="E32" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="G32" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
@@ -1061,10 +1090,16 @@
         <v>9</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -1075,16 +1110,19 @@
         <v>9</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="F34" s="0" t="s">
+        <v>12</v>
+      </c>
       <c r="G34" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1133,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,10 +1147,10 @@
         <v>9</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G36" s="0" t="s">
         <v>13</v>
@@ -1129,7 +1167,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,16 +1181,16 @@
         <v>9</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G38" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
@@ -1162,7 +1200,9 @@
       <c r="C39" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
@@ -1175,7 +1215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>7</v>
       </c>
@@ -1184,6 +1224,9 @@
       </c>
       <c r="C41" s="0" t="s">
         <v>9</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1194,6 +1237,53 @@
         <v>14</v>
       </c>
       <c r="C42" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#453 Minimum moves to equal array elements
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC089F6-3BCC-3A4E-82A7-C8AD575B703F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFD67B-F052-B645-96D0-637FDB6FF947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="70">
   <si>
     <t>Site</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>2020/12/28</t>
+  </si>
+  <si>
+    <t>453. Minimum Moves to Equal Array Elements</t>
+  </si>
+  <si>
+    <t>2021/01/21</t>
+  </si>
+  <si>
+    <t>Array, Large Integer, Sort</t>
   </si>
 </sst>
 </file>
@@ -260,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -273,6 +282,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1395,17 +1407,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" ht="28" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
@@ -1415,28 +1438,6 @@
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
practice: Solve Leetcode Problem#680 Valid Palindrome II
</commit_message>
<xml_diff>
--- a/Progress_Tracking.xlsx
+++ b/Progress_Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephangel/Desktop/Fun_Coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AFD67B-F052-B645-96D0-637FDB6FF947}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECEF11A-1791-AD43-B0FC-3D359C070178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="320" windowWidth="34180" windowHeight="16100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="74">
   <si>
     <t>Site</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>Array, Large Integer, Sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leetcode </t>
+  </si>
+  <si>
+    <t>680. Valid Palindrome II</t>
+  </si>
+  <si>
+    <t>2021/01/27</t>
+  </si>
+  <si>
+    <t>String, Boolean</t>
   </si>
 </sst>
 </file>
@@ -599,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39:G39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1407,38 +1419,75 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>